<commit_message>
added Calc Script and Plots
</commit_message>
<xml_diff>
--- a/Linear Regression Plot/LinAlgvScore.xlsx
+++ b/Linear Regression Plot/LinAlgvScore.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19F4A28-7276-481B-A7D5-3B62AA8ED485}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF7352B-337A-4E13-BD2F-579C81BB0727}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -388,7 +388,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F2" sqref="F2:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,30 +417,14 @@
       <c r="C2" s="2">
         <v>240</v>
       </c>
-      <c r="F2" s="3">
-        <v>82</v>
-      </c>
-      <c r="G2" s="1">
-        <v>77</v>
-      </c>
-      <c r="H2" s="1">
-        <v>80</v>
-      </c>
-      <c r="I2" s="1">
-        <v>90</v>
-      </c>
-      <c r="J2" s="3">
-        <v>86</v>
-      </c>
-      <c r="K2" s="1">
-        <v>79</v>
-      </c>
-      <c r="L2" s="3">
-        <v>77</v>
-      </c>
-      <c r="M2" s="3">
-        <v>72</v>
-      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -452,30 +436,14 @@
       <c r="C3" s="2">
         <v>144</v>
       </c>
-      <c r="F3" s="2">
-        <v>169</v>
-      </c>
-      <c r="G3" s="2">
-        <v>146</v>
-      </c>
-      <c r="H3" s="2">
-        <v>159</v>
-      </c>
-      <c r="I3" s="2">
-        <v>230</v>
-      </c>
-      <c r="J3" s="2">
-        <v>219</v>
-      </c>
-      <c r="K3" s="2">
-        <v>175</v>
-      </c>
-      <c r="L3" s="2">
-        <v>151</v>
-      </c>
-      <c r="M3" s="2">
-        <v>138</v>
-      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4">

</xml_diff>